<commit_message>
Finished PCB routing. Updated ESP32 GPIO layout.
</commit_message>
<xml_diff>
--- a/4_Docs/LizardBot1_ControlBoard_BOM.xlsx
+++ b/4_Docs/LizardBot1_ControlBoard_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
   <si>
     <t>Reference</t>
   </si>
@@ -351,7 +351,16 @@
     <t>C71370</t>
   </si>
   <si>
-    <t>J203,J204,J206,J502</t>
+    <t>J203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.54mm 2x3 (M)</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm:PinHeader_2x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>J502</t>
   </si>
   <si>
     <t>JST-S2B-PH-K-S(LF)(SN)</t>
@@ -366,7 +375,7 @@
     <t>C173752</t>
   </si>
   <si>
-    <t>J203-1,J204-1,J206-1,J502-1</t>
+    <t>J502-1</t>
   </si>
   <si>
     <t>JST-PHR-2</t>
@@ -1736,7 +1745,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="B40" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2335,137 +2344,134 @@
       <c r="B25" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>11</v>
-      </c>
+      <c r="C25" s="20"/>
       <c r="D25" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="E25" s="18">
-        <v>4</v>
-      </c>
+      <c r="E25" s="18"/>
       <c r="F25" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>115</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G25" s="19"/>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="E26" s="18">
+        <v>1</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="19" t="s">
+      <c r="H26" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="18"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="H27" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="E27" s="18">
-        <v>1</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="E28" s="18">
+        <v>1</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="19" t="s">
+      <c r="H28" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="C29" s="20"/>
+      <c r="D29" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="H29" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E29" s="18">
-        <v>1</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="E30" s="18">
+        <v>1</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="C30" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="17" t="s">
+      <c r="H30" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E30" s="18">
-        <v>2</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="1"/>
     </row>
     <row r="31" ht="14.25">
       <c r="A31" s="16" t="s">
@@ -2474,45 +2480,45 @@
       <c r="B31" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>132</v>
+      <c r="C31" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E31" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>135</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G31" s="1"/>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>11</v>
+        <v>143</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>135</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E32" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="33" ht="14.25">
       <c r="A33" s="16" t="s">
@@ -2528,207 +2534,207 @@
         <v>146</v>
       </c>
       <c r="E33" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>148</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G33" s="1"/>
     </row>
     <row r="34" ht="14.25">
       <c r="A34" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="E34" s="18">
+        <v>1</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="18"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="19" t="s">
+      <c r="H34" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="35" ht="14.25">
       <c r="A35" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="B35" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>11</v>
-      </c>
+      <c r="C35" s="17"/>
       <c r="D35" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="18"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="E35" s="18">
-        <v>3</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="36" ht="14.25">
       <c r="A36" s="16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="C36" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="D36" s="17" t="s">
-        <v>158</v>
-      </c>
       <c r="E36" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>160</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G36" s="1"/>
     </row>
     <row r="37" ht="14.25">
       <c r="A37" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="E37" s="18">
+        <v>1</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="H37" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E37" s="18">
-        <v>1</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="38" ht="14.25">
       <c r="A38" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E38" s="18">
+        <v>1</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="H38" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="I38" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="E38" s="18">
-        <v>1</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D39" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="E39" s="18">
+        <v>1</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="H39" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D39" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="E39" s="18">
-        <v>2</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G39" s="1"/>
     </row>
     <row r="40" ht="14.25">
       <c r="A40" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="C40" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="D40" s="17" t="s">
         <v>180</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>177</v>
       </c>
       <c r="E40" s="18">
         <v>2</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>182</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G40" s="1"/>
     </row>
     <row r="41" ht="14.25">
       <c r="A41" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="B41" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>11</v>
-      </c>
       <c r="D41" s="17" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E41" s="18">
         <v>2</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="G41" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="42" ht="14.25">
       <c r="A42" s="16" t="s">
@@ -2741,33 +2747,28 @@
         <v>11</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E42" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>189</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G42" s="1"/>
     </row>
     <row r="43" ht="14.25">
       <c r="A43" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B43" s="17" t="s">
         <v>190</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>191</v>
       </c>
       <c r="C43" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E43" s="18">
         <v>1</v>
@@ -2776,58 +2777,63 @@
         <v>13</v>
       </c>
       <c r="G43" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="44" ht="14.25">
       <c r="A44" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B44" s="17" t="s">
         <v>194</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>195</v>
       </c>
       <c r="C44" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E44" s="18">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F44" s="14" t="s">
         <v>13</v>
       </c>
       <c r="G44" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="45" ht="14.25">
       <c r="A45" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B45" s="17" t="s">
         <v>198</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>199</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D45" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="E45" s="18">
+        <v>6</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E45" s="18">
-        <v>4</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G45" s="1"/>
     </row>
     <row r="46" ht="14.25">
       <c r="A46" s="16" t="s">
@@ -2840,57 +2846,57 @@
         <v>11</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="E46" s="18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>204</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G46" s="1"/>
     </row>
     <row r="47" ht="14.25">
       <c r="A47" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B47" s="17" t="s">
         <v>205</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>195</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="E47" s="18">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G47" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="G47" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="48" ht="14.25">
       <c r="A48" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B48" s="17">
-        <v>470</v>
+        <v>208</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>198</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E48" s="18">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F48" s="14" t="s">
         <v>19</v>
@@ -2899,162 +2905,157 @@
     </row>
     <row r="49" ht="14.25">
       <c r="A49" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>208</v>
+        <v>209</v>
+      </c>
+      <c r="B49" s="17">
+        <v>470</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E49" s="18">
         <v>2</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G49" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>210</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G49" s="1"/>
     </row>
     <row r="50" ht="14.25">
       <c r="A50" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>211</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>212</v>
       </c>
       <c r="C50" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E50" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G50" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="G50" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="51" ht="14.25">
       <c r="A51" s="16" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C51" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="E51" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>216</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G51" s="1"/>
     </row>
     <row r="52" ht="14.25">
       <c r="A52" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="B52" s="17" t="s">
         <v>217</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>218</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E52" s="18">
         <v>1</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G52" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="G52" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="53" ht="14.25">
       <c r="A53" s="16" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C53" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E53" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>222</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G53" s="1"/>
     </row>
     <row r="54" ht="14.25">
       <c r="A54" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" s="17" t="s">
         <v>223</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>224</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E54" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F54" s="14" t="s">
         <v>13</v>
       </c>
       <c r="G54" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="55" ht="14.25">
       <c r="A55" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B55" s="17" t="s">
         <v>227</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>228</v>
       </c>
       <c r="C55" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E55" s="18">
         <v>1</v>
@@ -3063,48 +3064,53 @@
         <v>13</v>
       </c>
       <c r="G55" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="56" ht="14.25">
       <c r="A56" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="B56" s="17" t="s">
         <v>231</v>
-      </c>
-      <c r="B56" s="17">
-        <v>150</v>
       </c>
       <c r="C56" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E56" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G56" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="G56" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="57" ht="14.25">
       <c r="A57" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>233</v>
+        <v>234</v>
+      </c>
+      <c r="B57" s="17">
+        <v>150</v>
       </c>
       <c r="C57" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>234</v>
+        <v>188</v>
       </c>
       <c r="E57" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F57" s="14" t="s">
         <v>19</v>
@@ -3125,7 +3131,7 @@
         <v>237</v>
       </c>
       <c r="E58" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" s="14" t="s">
         <v>19</v>
@@ -3143,10 +3149,10 @@
         <v>11</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="E59" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F59" s="14" t="s">
         <v>19</v>
@@ -3155,16 +3161,16 @@
     </row>
     <row r="60" ht="14.25">
       <c r="A60" s="16" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C60" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E60" s="18">
         <v>1</v>
@@ -3176,239 +3182,252 @@
     </row>
     <row r="61" ht="14.25">
       <c r="A61" s="16" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="C61" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="D61" s="17" t="s">
-        <v>245</v>
-      </c>
       <c r="E61" s="18">
         <v>1</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G61" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>248</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G61" s="1"/>
     </row>
     <row r="62" ht="14.25">
       <c r="A62" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="E62" s="18">
+        <v>1</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="B62" s="17" t="s">
+      <c r="H62" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="I62" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="D62" s="17" t="s">
-        <v>252</v>
-      </c>
-      <c r="E62" s="18">
-        <v>1</v>
-      </c>
-      <c r="F62" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G62" s="19" t="s">
-        <v>253</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="63" ht="14.25">
       <c r="A63" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="D63" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="E63" s="18">
+        <v>1</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="C63" s="20" t="s">
+      <c r="H63" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>258</v>
-      </c>
-      <c r="E63" s="18">
-        <v>1</v>
-      </c>
-      <c r="F63" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G63" s="19" t="s">
-        <v>259</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="64" ht="14.25">
       <c r="A64" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="E64" s="18">
+        <v>1</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G64" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="H64" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="I64" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>265</v>
-      </c>
-      <c r="E64" s="18">
-        <v>1</v>
-      </c>
-      <c r="F64" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G64" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="65" ht="14.25">
       <c r="A65" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="D65" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="E65" s="18">
+        <v>1</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="H65" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>271</v>
-      </c>
-      <c r="E65" s="18">
-        <v>1</v>
-      </c>
-      <c r="F65" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G65" s="19" t="s">
-        <v>272</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="66" ht="14.25">
       <c r="A66" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="D66" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="E66" s="18">
+        <v>1</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G66" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="H66" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="D66" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="E66" s="18">
-        <v>2</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G66" s="19" t="s">
-        <v>278</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="67" ht="14.25">
       <c r="A67" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="D67" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="E67" s="18">
+        <v>2</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="H67" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D67" s="17" t="s">
+    </row>
+    <row r="68" ht="14.25">
+      <c r="A68" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="E67" s="18">
-        <v>1</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G67" s="19" t="s">
+      <c r="B68" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="H67" s="1" t="s">
+      <c r="C68" s="20" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="68" ht="14.25">
-      <c r="A68" s="21" t="s">
+      <c r="D68" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="B68" s="22" t="s">
+      <c r="E68" s="18">
+        <v>1</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="19" t="s">
         <v>287</v>
       </c>
-      <c r="C68" s="23" t="s">
+      <c r="H68" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D68" s="22" t="s">
+    </row>
+    <row r="69" ht="14.25">
+      <c r="A69" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="E68" s="24">
-        <v>1</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G68" s="19" t="s">
+      <c r="B69" s="22" t="s">
         <v>290</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="C69" s="23" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="69" ht="14.25">
-      <c r="A69" s="25" t="s">
+      <c r="D69" s="22" t="s">
         <v>292</v>
       </c>
-      <c r="B69" s="26"/>
-      <c r="C69" s="26"/>
-      <c r="D69" s="26"/>
-      <c r="E69" s="27">
-        <f>SUM(E2:E68)</f>
-        <v>126</v>
-      </c>
-      <c r="F69" s="4"/>
-      <c r="G69" s="1"/>
+      <c r="E69" s="24">
+        <v>1</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G69" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="70" ht="14.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="3"/>
+      <c r="A70" s="25" t="s">
+        <v>295</v>
+      </c>
+      <c r="B70" s="26"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="27">
+        <f>SUM(E2:E69)</f>
+        <v>123</v>
+      </c>
       <c r="F70" s="4"/>
+      <c r="G70" s="1"/>
     </row>
     <row r="71" ht="14.25">
       <c r="A71" s="1"/>
@@ -3451,14 +3470,22 @@
       <c r="F75" s="4"/>
     </row>
     <row r="76" ht="14.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="3"/>
       <c r="F76" s="4"/>
     </row>
     <row r="77" ht="14.25">
       <c r="F77" s="4"/>
     </row>
+    <row r="78" ht="14.25">
+      <c r="F78" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A70:D70"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="G2"/>
@@ -3484,51 +3511,51 @@
     <hyperlink r:id="rId21" ref="C23"/>
     <hyperlink r:id="rId22" ref="G23"/>
     <hyperlink r:id="rId23" ref="G24"/>
-    <hyperlink r:id="rId24" ref="G25"/>
-    <hyperlink r:id="rId25" ref="G26"/>
-    <hyperlink r:id="rId26" ref="C27"/>
-    <hyperlink r:id="rId27" ref="G27"/>
-    <hyperlink r:id="rId28" ref="G28"/>
-    <hyperlink r:id="rId29" ref="C29"/>
-    <hyperlink r:id="rId30" ref="G29"/>
-    <hyperlink r:id="rId29" ref="C31"/>
-    <hyperlink r:id="rId30" ref="G31"/>
-    <hyperlink r:id="rId31" ref="G33"/>
-    <hyperlink r:id="rId32" ref="G34"/>
-    <hyperlink r:id="rId33" ref="C36"/>
-    <hyperlink r:id="rId34" ref="G36"/>
-    <hyperlink r:id="rId35" ref="C37"/>
-    <hyperlink r:id="rId36" ref="G37"/>
-    <hyperlink r:id="rId37" ref="C38"/>
-    <hyperlink r:id="rId38" ref="G38"/>
-    <hyperlink r:id="rId39" ref="C39"/>
-    <hyperlink r:id="rId40" ref="C40"/>
-    <hyperlink r:id="rId41" ref="G40"/>
-    <hyperlink r:id="rId42" ref="G42"/>
-    <hyperlink r:id="rId43" ref="G43"/>
-    <hyperlink r:id="rId44" ref="G44"/>
-    <hyperlink r:id="rId45" ref="G46"/>
-    <hyperlink r:id="rId46" ref="G49"/>
-    <hyperlink r:id="rId47" ref="G51"/>
-    <hyperlink r:id="rId48" ref="G53"/>
-    <hyperlink r:id="rId49" ref="G54"/>
-    <hyperlink r:id="rId50" ref="G55"/>
-    <hyperlink r:id="rId51" ref="C61"/>
-    <hyperlink r:id="rId52" ref="G61"/>
-    <hyperlink r:id="rId53" ref="C62"/>
-    <hyperlink r:id="rId54" ref="G62"/>
-    <hyperlink r:id="rId55" ref="C63"/>
-    <hyperlink r:id="rId56" ref="G63"/>
-    <hyperlink r:id="rId57" ref="C64"/>
-    <hyperlink r:id="rId58" ref="G64"/>
-    <hyperlink r:id="rId59" ref="C65"/>
-    <hyperlink r:id="rId60" ref="G65"/>
-    <hyperlink r:id="rId61" ref="C66"/>
-    <hyperlink r:id="rId62" ref="G66"/>
-    <hyperlink r:id="rId63" ref="C67"/>
-    <hyperlink r:id="rId64" ref="G67"/>
-    <hyperlink r:id="rId65" ref="C68"/>
-    <hyperlink r:id="rId66" ref="G68"/>
+    <hyperlink r:id="rId24" ref="G26"/>
+    <hyperlink r:id="rId25" ref="G27"/>
+    <hyperlink r:id="rId26" ref="C28"/>
+    <hyperlink r:id="rId27" ref="G28"/>
+    <hyperlink r:id="rId28" ref="G29"/>
+    <hyperlink r:id="rId29" ref="C30"/>
+    <hyperlink r:id="rId30" ref="G30"/>
+    <hyperlink r:id="rId29" ref="C32"/>
+    <hyperlink r:id="rId30" ref="G32"/>
+    <hyperlink r:id="rId31" ref="G34"/>
+    <hyperlink r:id="rId32" ref="G35"/>
+    <hyperlink r:id="rId33" ref="C37"/>
+    <hyperlink r:id="rId34" ref="G37"/>
+    <hyperlink r:id="rId35" ref="C38"/>
+    <hyperlink r:id="rId36" ref="G38"/>
+    <hyperlink r:id="rId37" ref="C39"/>
+    <hyperlink r:id="rId38" ref="G39"/>
+    <hyperlink r:id="rId39" ref="C40"/>
+    <hyperlink r:id="rId40" ref="C41"/>
+    <hyperlink r:id="rId41" ref="G41"/>
+    <hyperlink r:id="rId42" ref="G43"/>
+    <hyperlink r:id="rId43" ref="G44"/>
+    <hyperlink r:id="rId44" ref="G45"/>
+    <hyperlink r:id="rId45" ref="G47"/>
+    <hyperlink r:id="rId46" ref="G50"/>
+    <hyperlink r:id="rId47" ref="G52"/>
+    <hyperlink r:id="rId48" ref="G54"/>
+    <hyperlink r:id="rId49" ref="G55"/>
+    <hyperlink r:id="rId50" ref="G56"/>
+    <hyperlink r:id="rId51" ref="C62"/>
+    <hyperlink r:id="rId52" ref="G62"/>
+    <hyperlink r:id="rId53" ref="C63"/>
+    <hyperlink r:id="rId54" ref="G63"/>
+    <hyperlink r:id="rId55" ref="C64"/>
+    <hyperlink r:id="rId56" ref="G64"/>
+    <hyperlink r:id="rId57" ref="C65"/>
+    <hyperlink r:id="rId58" ref="G65"/>
+    <hyperlink r:id="rId59" ref="C66"/>
+    <hyperlink r:id="rId60" ref="G66"/>
+    <hyperlink r:id="rId61" ref="C67"/>
+    <hyperlink r:id="rId62" ref="G67"/>
+    <hyperlink r:id="rId63" ref="C68"/>
+    <hyperlink r:id="rId64" ref="G68"/>
+    <hyperlink r:id="rId65" ref="C69"/>
+    <hyperlink r:id="rId66" ref="G69"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -3538,7 +3565,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{008300E5-0031-4412-87EC-0004001E003B}">
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{00F1008B-0007-4C49-B668-002400E400F6}">
             <xm:f>"YES"</xm:f>
             <x14:dxf>
               <font>
@@ -3555,7 +3582,7 @@
           <xm:sqref>F:F</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00C500AF-00CE-406B-8C3B-002D00E80080}">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00BA00E9-0011-4BAD-A9C7-00C2001900CF}">
             <xm:f>"NO"</xm:f>
             <x14:dxf>
               <font>
@@ -3571,6 +3598,40 @@
           </x14:cfRule>
           <xm:sqref>F:F</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{009300FA-00E0-4C33-998C-00B700420046}">
+            <xm:f>"YES"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00000077-00A7-470A-AA32-00C300A30066}">
+            <xm:f>"NO"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F25</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Finished robot controller PCB. Generated production files.
</commit_message>
<xml_diff>
--- a/4_Docs/LizardBot1_ControlBoard_BOM.xlsx
+++ b/4_Docs/LizardBot1_ControlBoard_BOM.xlsx
@@ -3,10 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Quote" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="318">
   <si>
     <t>Reference</t>
   </si>
@@ -231,7 +232,7 @@
     <t>C2760101</t>
   </si>
   <si>
-    <t xml:space="preserve">No stock at LCSC. Mouser: 576-0PTF0078P.</t>
+    <t xml:space="preserve">No stock at LCSC. Mouser: 576-0PTF0078P</t>
   </si>
   <si>
     <t>F201-1</t>
@@ -246,7 +247,7 @@
     <t>C5299837</t>
   </si>
   <si>
-    <t xml:space="preserve">Low stock at LCSC. Mouser: 576-00BS0232P.</t>
+    <t xml:space="preserve">Low stock at LCSC. Mouser: 576-00BS0232P</t>
   </si>
   <si>
     <t>F201-2</t>
@@ -258,7 +259,7 @@
     <t>C3166596</t>
   </si>
   <si>
-    <t xml:space="preserve">No stock at LCSC. Mouser: 0234010.MXP.</t>
+    <t xml:space="preserve">No stock at LCSC. Mouser: 0234010.MXP</t>
   </si>
   <si>
     <t>F202</t>
@@ -435,6 +436,9 @@
     <t>C7095263</t>
   </si>
   <si>
+    <t xml:space="preserve">No stock at LCSC. Mouser: 640-USB4085-GF-A</t>
+  </si>
+  <si>
     <t>J301,J302</t>
   </si>
   <si>
@@ -528,9 +532,6 @@
     <t>C6495636</t>
   </si>
   <si>
-    <t xml:space="preserve">Edit footprint pin number in KiCad!</t>
-  </si>
-  <si>
     <t>Q301</t>
   </si>
   <si>
@@ -771,7 +772,7 @@
     <t>946-MP2225GJ-Z</t>
   </si>
   <si>
-    <t xml:space="preserve">Discontinued at LCSC! Mouser: 946-MP2225GJ-Z.</t>
+    <t xml:space="preserve">Discontinued at LCSC! Mouser: 946-MP2225GJ-Z</t>
   </si>
   <si>
     <t>U202</t>
@@ -810,7 +811,7 @@
     <t>356-ESP32WRM32E164PH</t>
   </si>
   <si>
-    <t xml:space="preserve">More expensive from LCSC. Order from Mouser: 356-ESP32WRM32E164PH.</t>
+    <t xml:space="preserve">More expensive from LCSC. Order from Mouser: 356-ESP32WRM32E164PH</t>
   </si>
   <si>
     <t>U302</t>
@@ -849,6 +850,9 @@
     <t>C969151</t>
   </si>
   <si>
+    <t xml:space="preserve">Order in PCBA</t>
+  </si>
+  <si>
     <t>U401,U402</t>
   </si>
   <si>
@@ -885,6 +889,9 @@
     <t>C510894</t>
   </si>
   <si>
+    <t xml:space="preserve">No stock at LCSC. Mouser: 998-MIC5225-1.8YM5TR</t>
+  </si>
+  <si>
     <t>U502</t>
   </si>
   <si>
@@ -904,12 +911,75 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB &amp; Assembly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrival in 12-15 business days.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Original Balance</t>
+  </si>
+  <si>
+    <t>LCSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB Parts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrival in 7-15 business days.</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB Parts &amp; Lidar &amp; Raspberry Kit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrival in 2-3 business days.</t>
+  </si>
+  <si>
+    <t>Mauser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry Pi 4B 4GB Kit</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Motors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery &amp; Charger</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+  </numFmts>
   <fonts count="8">
     <font>
       <sz val="11.000000"/>
@@ -957,12 +1027,27 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="5"/>
+        <bgColor indexed="5"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="14">
@@ -1155,10 +1240,11 @@
       <diagonal style="none"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="48">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1201,6 +1287,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="5" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1214,6 +1301,7 @@
     <xf fontId="6" fillId="0" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf fontId="1" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="5" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1235,9 +1323,44 @@
     <xf fontId="1" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="16" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="16" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1745,7 +1868,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B46" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1814,24 +1937,24 @@
       <c r="G2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="19">
         <v>5</v>
       </c>
       <c r="F3" s="14" t="s">
@@ -1840,19 +1963,19 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="19">
         <v>5</v>
       </c>
       <c r="F4" s="14" t="s">
@@ -1861,19 +1984,19 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="19">
         <v>14</v>
       </c>
       <c r="F5" s="14" t="s">
@@ -1882,45 +2005,45 @@
       <c r="G5" s="1"/>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="19">
         <v>1</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="16" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="19">
         <v>1</v>
       </c>
       <c r="F7" s="14" t="s">
@@ -1929,24 +2052,24 @@
       <c r="G7" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="16" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="19">
         <v>6</v>
       </c>
       <c r="F8" s="14" t="s">
@@ -1955,19 +2078,19 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="19">
         <v>2</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -1976,76 +2099,76 @@
       <c r="G9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="19">
         <v>2</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="16" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="19">
         <v>1</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="19">
         <v>3</v>
       </c>
       <c r="F12" s="14" t="s">
@@ -2054,45 +2177,45 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="19">
         <v>1</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="19">
         <v>1</v>
       </c>
       <c r="F14" s="14" t="s">
@@ -2101,19 +2224,19 @@
       <c r="G14" s="1"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="19">
         <v>2</v>
       </c>
       <c r="F15" s="14" t="s">
@@ -2122,28 +2245,28 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="19">
         <v>1</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="16" t="s">
         <v>70</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -2151,20 +2274,20 @@
       </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="17" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="18"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="14"/>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="22" t="s">
         <v>75</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -2172,20 +2295,20 @@
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="17" t="s">
+      <c r="B18" s="18"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="18"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="14"/>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="16" t="s">
         <v>79</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -2193,71 +2316,71 @@
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="19">
         <v>1</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="16" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="19">
         <v>1</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="16" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="19">
         <v>1</v>
       </c>
       <c r="F21" s="14" t="s">
@@ -2266,227 +2389,230 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="19">
         <v>1</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="16" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="19">
         <v>1</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" s="16" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="17" t="s">
+      <c r="C24" s="21"/>
+      <c r="D24" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="18"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="16" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="17" t="s">
+      <c r="C25" s="21"/>
+      <c r="D25" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="E25" s="18"/>
+      <c r="E25" s="19"/>
       <c r="F25" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="19"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="19">
         <v>1</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="19" t="s">
+      <c r="G26" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="16" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17" t="s">
+      <c r="C27" s="18"/>
+      <c r="D27" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E27" s="18"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="14"/>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" s="16" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28" s="19">
         <v>1</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="19" t="s">
+      <c r="G28" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="16" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="17" t="s">
+      <c r="C29" s="21"/>
+      <c r="D29" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="18"/>
+      <c r="E29" s="19"/>
       <c r="F29" s="14"/>
-      <c r="G29" s="19" t="s">
+      <c r="G29" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="16" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30" s="19">
         <v>1</v>
       </c>
       <c r="F30" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="19" t="s">
+      <c r="G30" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" s="22" t="s">
         <v>138</v>
       </c>
+      <c r="I30" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B31" s="17" t="s">
+      <c r="A31" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="B31" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="E31" s="18">
+      <c r="D31" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E31" s="19">
         <v>2</v>
       </c>
       <c r="F31" s="14" t="s">
@@ -2495,45 +2621,48 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="B32" s="17" t="s">
+      <c r="A32" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="B32" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32" s="19">
         <v>1</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="19" t="s">
+      <c r="G32" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H32" s="22" t="s">
         <v>138</v>
       </c>
+      <c r="I32" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="B33" s="17" t="s">
+      <c r="A33" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="B33" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="E33" s="18">
+      <c r="D33" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E33" s="19">
         <v>2</v>
       </c>
       <c r="F33" s="14" t="s">
@@ -2542,65 +2671,65 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" s="17" t="s">
+      <c r="A34" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="B34" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="E34" s="18">
+      <c r="D34" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="19">
         <v>1</v>
       </c>
       <c r="F34" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G34" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="H34" s="1" t="s">
+      <c r="G34" s="20" t="s">
         <v>151</v>
       </c>
+      <c r="H34" s="16" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="B35" s="17" t="s">
+      <c r="A35" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17" t="s">
+      <c r="B35" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E35" s="18"/>
+      <c r="E35" s="19"/>
       <c r="F35" s="14"/>
-      <c r="G35" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="H35" s="1" t="s">
+      <c r="G35" s="20" t="s">
         <v>155</v>
       </c>
+      <c r="H35" s="16" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="C36" s="17" t="s">
+      <c r="A36" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="E36" s="18">
+      <c r="D36" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="E36" s="19">
         <v>3</v>
       </c>
       <c r="F36" s="14" t="s">
@@ -2609,100 +2738,98 @@
       <c r="G36" s="1"/>
     </row>
     <row r="37" ht="14.25">
-      <c r="A37" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="B37" s="17" t="s">
+      <c r="A37" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="B37" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="C37" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="E37" s="18">
+      <c r="D37" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E37" s="19">
         <v>1</v>
       </c>
       <c r="F37" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="H37" s="1" t="s">
+      <c r="G37" s="20" t="s">
         <v>163</v>
       </c>
+      <c r="H37" s="16" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="38" ht="14.25">
-      <c r="A38" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="B38" s="17" t="s">
+      <c r="A38" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="C38" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="E38" s="18">
+      <c r="D38" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="E38" s="19">
         <v>1</v>
       </c>
       <c r="F38" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="H38" s="1" t="s">
+      <c r="G38" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="H38" s="16" t="s">
         <v>170</v>
       </c>
+      <c r="I38" s="1"/>
     </row>
     <row r="39" ht="14.25">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="19">
         <v>1</v>
       </c>
       <c r="F39" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G39" s="19" t="s">
+      <c r="G39" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" s="16" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="40" ht="14.25">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="E40" s="18">
+      <c r="E40" s="19">
         <v>2</v>
       </c>
       <c r="F40" s="14" t="s">
@@ -2711,45 +2838,45 @@
       <c r="G40" s="1"/>
     </row>
     <row r="41" ht="14.25">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="E41" s="18">
+      <c r="E41" s="19">
         <v>2</v>
       </c>
       <c r="F41" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G41" s="19" t="s">
+      <c r="G41" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H41" s="16" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="42" ht="14.25">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D42" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="E42" s="18">
+      <c r="E42" s="19">
         <v>2</v>
       </c>
       <c r="F42" s="14" t="s">
@@ -2758,97 +2885,97 @@
       <c r="G42" s="1"/>
     </row>
     <row r="43" ht="14.25">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="E43" s="18">
+      <c r="E43" s="19">
         <v>1</v>
       </c>
       <c r="F43" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G43" s="19" t="s">
+      <c r="G43" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H43" s="16" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="44" ht="14.25">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="E44" s="18">
+      <c r="E44" s="19">
         <v>1</v>
       </c>
       <c r="F44" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G44" s="19" t="s">
+      <c r="G44" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H44" s="16" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="45" ht="14.25">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D45" s="17" t="s">
+      <c r="D45" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="E45" s="18">
+      <c r="E45" s="19">
         <v>6</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G45" s="19" t="s">
+      <c r="G45" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H45" s="16" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="46" ht="14.25">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="D46" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="E46" s="18">
+      <c r="E46" s="19">
         <v>4</v>
       </c>
       <c r="F46" s="14" t="s">
@@ -2857,45 +2984,45 @@
       <c r="G46" s="1"/>
     </row>
     <row r="47" ht="14.25">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="E47" s="18">
+      <c r="E47" s="19">
         <v>1</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G47" s="19" t="s">
+      <c r="G47" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" s="16" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="48" ht="14.25">
-      <c r="A48" s="16" t="s">
+      <c r="A48" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="17" t="s">
+      <c r="D48" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="E48" s="18">
+      <c r="E48" s="19">
         <v>9</v>
       </c>
       <c r="F48" s="14" t="s">
@@ -2904,19 +3031,19 @@
       <c r="G48" s="1"/>
     </row>
     <row r="49" ht="14.25">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="B49" s="17">
+      <c r="B49" s="18">
         <v>470</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="C49" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D49" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="E49" s="18">
+      <c r="E49" s="19">
         <v>2</v>
       </c>
       <c r="F49" s="14" t="s">
@@ -2925,45 +3052,45 @@
       <c r="G49" s="1"/>
     </row>
     <row r="50" ht="14.25">
-      <c r="A50" s="16" t="s">
+      <c r="A50" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="D50" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="E50" s="18">
+      <c r="E50" s="19">
         <v>2</v>
       </c>
       <c r="F50" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G50" s="19" t="s">
+      <c r="G50" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="H50" s="16" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="51" ht="14.25">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="C51" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="17" t="s">
+      <c r="D51" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="E51" s="18">
+      <c r="E51" s="19">
         <v>3</v>
       </c>
       <c r="F51" s="14" t="s">
@@ -2972,45 +3099,45 @@
       <c r="G51" s="1"/>
     </row>
     <row r="52" ht="14.25">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C52" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="17" t="s">
+      <c r="D52" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="E52" s="18">
+      <c r="E52" s="19">
         <v>1</v>
       </c>
       <c r="F52" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G52" s="19" t="s">
+      <c r="G52" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="H52" s="16" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="53" ht="14.25">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C53" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D53" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="E53" s="18">
+      <c r="E53" s="19">
         <v>1</v>
       </c>
       <c r="F53" s="14" t="s">
@@ -3019,97 +3146,97 @@
       <c r="G53" s="1"/>
     </row>
     <row r="54" ht="14.25">
-      <c r="A54" s="16" t="s">
+      <c r="A54" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D54" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="E54" s="18">
+      <c r="E54" s="19">
         <v>2</v>
       </c>
       <c r="F54" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G54" s="19" t="s">
+      <c r="G54" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="H54" s="16" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="55" ht="14.25">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C55" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="17" t="s">
+      <c r="D55" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="E55" s="18">
+      <c r="E55" s="19">
         <v>1</v>
       </c>
       <c r="F55" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G55" s="19" t="s">
+      <c r="G55" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="H55" s="16" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="56" ht="14.25">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C56" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D56" s="17" t="s">
+      <c r="D56" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="E56" s="18">
+      <c r="E56" s="19">
         <v>1</v>
       </c>
       <c r="F56" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G56" s="19" t="s">
+      <c r="G56" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="H56" s="16" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="57" ht="14.25">
-      <c r="A57" s="16" t="s">
+      <c r="A57" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="B57" s="17">
+      <c r="B57" s="18">
         <v>150</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="C57" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="17" t="s">
+      <c r="D57" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="E57" s="18">
+      <c r="E57" s="19">
         <v>2</v>
       </c>
       <c r="F57" s="14" t="s">
@@ -3118,19 +3245,19 @@
       <c r="G57" s="1"/>
     </row>
     <row r="58" ht="14.25">
-      <c r="A58" s="16" t="s">
+      <c r="A58" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="C58" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D58" s="17" t="s">
+      <c r="D58" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="E58" s="18">
+      <c r="E58" s="19">
         <v>1</v>
       </c>
       <c r="F58" s="14" t="s">
@@ -3139,19 +3266,19 @@
       <c r="G58" s="1"/>
     </row>
     <row r="59" ht="14.25">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="C59" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D59" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="E59" s="18">
+      <c r="E59" s="19">
         <v>2</v>
       </c>
       <c r="F59" s="14" t="s">
@@ -3160,19 +3287,19 @@
       <c r="G59" s="1"/>
     </row>
     <row r="60" ht="14.25">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="17" t="s">
+      <c r="D60" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="E60" s="18">
+      <c r="E60" s="19">
         <v>1</v>
       </c>
       <c r="F60" s="14" t="s">
@@ -3181,19 +3308,19 @@
       <c r="G60" s="1"/>
     </row>
     <row r="61" ht="14.25">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="C61" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D61" s="17" t="s">
+      <c r="D61" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="E61" s="18">
+      <c r="E61" s="19">
         <v>1</v>
       </c>
       <c r="F61" s="14" t="s">
@@ -3202,28 +3329,28 @@
       <c r="G61" s="1"/>
     </row>
     <row r="62" ht="14.25">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="B62" s="17" t="s">
+      <c r="B62" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="C62" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="E62" s="18">
+      <c r="E62" s="19">
         <v>1</v>
       </c>
       <c r="F62" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G62" s="19" t="s">
+      <c r="G62" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="H62" s="1" t="s">
+      <c r="H62" s="22" t="s">
         <v>250</v>
       </c>
       <c r="I62" s="1" t="s">
@@ -3231,54 +3358,54 @@
       </c>
     </row>
     <row r="63" ht="14.25">
-      <c r="A63" s="16" t="s">
+      <c r="A63" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B63" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="C63" s="20" t="s">
+      <c r="C63" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="D63" s="17" t="s">
+      <c r="D63" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="E63" s="18">
+      <c r="E63" s="19">
         <v>1</v>
       </c>
       <c r="F63" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G63" s="19" t="s">
+      <c r="G63" s="20" t="s">
         <v>256</v>
       </c>
-      <c r="H63" s="1" t="s">
+      <c r="H63" s="16" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="64" ht="14.25">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="D64" s="17" t="s">
+      <c r="D64" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="E64" s="18">
+      <c r="E64" s="19">
         <v>1</v>
       </c>
       <c r="F64" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G64" s="19" t="s">
+      <c r="G64" s="20" t="s">
         <v>262</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="H64" s="22" t="s">
         <v>263</v>
       </c>
       <c r="I64" s="1" t="s">
@@ -3286,143 +3413,152 @@
       </c>
     </row>
     <row r="65" ht="14.25">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="D65" s="17" t="s">
+      <c r="D65" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="E65" s="18">
+      <c r="E65" s="19">
         <v>1</v>
       </c>
       <c r="F65" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G65" s="19" t="s">
+      <c r="G65" s="20" t="s">
         <v>269</v>
       </c>
-      <c r="H65" s="1" t="s">
+      <c r="H65" s="16" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="66" ht="14.25">
-      <c r="A66" s="16" t="s">
+      <c r="A66" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="D66" s="17" t="s">
+      <c r="D66" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="E66" s="18">
+      <c r="E66" s="19">
         <v>1</v>
       </c>
       <c r="F66" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G66" s="19" t="s">
+      <c r="G66" s="20" t="s">
         <v>275</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>276</v>
       </c>
+      <c r="I66" s="1" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="67" ht="14.25">
-      <c r="A67" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="B67" s="17" t="s">
+      <c r="A67" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="B67" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="D67" s="17" t="s">
+      <c r="C67" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="E67" s="18">
+      <c r="D67" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="E67" s="19">
         <v>2</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G67" s="19" t="s">
-        <v>281</v>
-      </c>
-      <c r="H67" s="1" t="s">
+      <c r="G67" s="20" t="s">
         <v>282</v>
       </c>
+      <c r="H67" s="16" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="68" ht="14.25">
-      <c r="A68" s="16" t="s">
-        <v>283</v>
-      </c>
-      <c r="B68" s="17" t="s">
+      <c r="A68" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="B68" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="D68" s="17" t="s">
+      <c r="C68" s="21" t="s">
         <v>286</v>
       </c>
-      <c r="E68" s="18">
+      <c r="D68" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="E68" s="19">
         <v>1</v>
       </c>
       <c r="F68" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G68" s="19" t="s">
-        <v>287</v>
-      </c>
-      <c r="H68" s="1" t="s">
+      <c r="G68" s="20" t="s">
         <v>288</v>
       </c>
+      <c r="H68" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="69" ht="14.25">
-      <c r="A69" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="B69" s="22" t="s">
-        <v>290</v>
-      </c>
-      <c r="C69" s="23" t="s">
+      <c r="A69" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="D69" s="22" t="s">
+      <c r="B69" s="24" t="s">
         <v>292</v>
       </c>
-      <c r="E69" s="24">
+      <c r="C69" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="D69" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="E69" s="26">
         <v>1</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G69" s="19" t="s">
-        <v>293</v>
+      <c r="G69" s="20" t="s">
+        <v>295</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="70" ht="14.25">
-      <c r="A70" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="B70" s="26"/>
-      <c r="C70" s="26"/>
-      <c r="D70" s="26"/>
-      <c r="E70" s="27">
+      <c r="A70" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="B70" s="28"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="28"/>
+      <c r="E70" s="29">
         <f>SUM(E2:E69)</f>
         <v>123</v>
       </c>
@@ -3565,7 +3701,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{00F1008B-0007-4C49-B668-002400E400F6}">
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{00EF00B1-0095-464B-9196-000B007D00E6}">
             <xm:f>"YES"</xm:f>
             <x14:dxf>
               <font>
@@ -3582,7 +3718,24 @@
           <xm:sqref>F:F</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00BA00E9-0011-4BAD-A9C7-00C2001900CF}">
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{004800B2-001D-411D-BC48-00F500D80023}">
+            <xm:f>"YES"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00900089-0049-4040-A86C-000200F80032}">
             <xm:f>"NO"</xm:f>
             <x14:dxf>
               <font>
@@ -3599,24 +3752,7 @@
           <xm:sqref>F:F</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{009300FA-00E0-4C33-998C-00B700420046}">
-            <xm:f>"YES"</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>F25</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00000077-00A7-470A-AA32-00C300A30066}">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{0094003E-0044-41AD-9BD8-00B3002500A2}">
             <xm:f>"NO"</xm:f>
             <x14:dxf>
               <font>
@@ -3636,4 +3772,157 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="2" max="2" width="29.47265625"/>
+    <col min="3" max="4" style="30" width="9.140625"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="31" width="28.23046875"/>
+    <col bestFit="1" min="7" max="7" width="14.61328125"/>
+    <col bestFit="1" min="8" max="9" width="10.90234375"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>300</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>301</v>
+      </c>
+      <c r="H1" s="30">
+        <f>SUM(C:C)</f>
+        <v>350.29999999999995</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="34" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>303</v>
+      </c>
+      <c r="C2" s="36">
+        <v>105.51000000000001</v>
+      </c>
+      <c r="D2" s="37">
+        <v>45513</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>304</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="H2" s="30">
+        <v>3253.9499999999998</v>
+      </c>
+      <c r="J2" s="30"/>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" s="41">
+        <v>43.719999999999999</v>
+      </c>
+      <c r="D3" s="42">
+        <v>45513</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>308</v>
+      </c>
+      <c r="G3" s="43" t="s">
+        <v>309</v>
+      </c>
+      <c r="H3" s="44">
+        <f>H2-H1</f>
+        <v>2903.6499999999996</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>311</v>
+      </c>
+      <c r="C4" s="30">
+        <v>102.14</v>
+      </c>
+      <c r="D4" s="46">
+        <v>45520</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>314</v>
+      </c>
+      <c r="C5" s="30">
+        <v>77.909999999999997</v>
+      </c>
+      <c r="D5" s="46">
+        <v>45520</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>316</v>
+      </c>
+      <c r="C6" s="30">
+        <v>21.02</v>
+      </c>
+      <c r="D6" s="46">
+        <v>45520</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="B7" t="s">
+        <v>317</v>
+      </c>
+      <c r="E7" s="31"/>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>